<commit_message>
Added As(III) data to original ICP totals dataset
Only added columns from As speciation data set to the total ICP dataset
to calculate the sum of electrons transfered to As, Fe, and Mn
</commit_message>
<xml_diff>
--- a/Aggregate_AqMnAsFe.xlsx
+++ b/Aggregate_AqMnAsFe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="380" windowWidth="28600" windowHeight="20340" tabRatio="500"/>
+    <workbookView xWindow="820" yWindow="1420" windowWidth="28360" windowHeight="20160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>As_uM_A</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,6 +82,22 @@
   </si>
   <si>
     <t>Mn_uM_3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>As3_uM_A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>As3_uM_B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>As3_uM_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>As3_uM_3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -456,15 +472,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:P32"/>
+  <dimension ref="A1:U32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:21">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -472,49 +488,61 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="P1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="R1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="S1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="U1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:21">
       <c r="A2">
         <v>1</v>
       </c>
@@ -522,49 +550,61 @@
         <v>72.013000000000005</v>
       </c>
       <c r="C2">
+        <v>25.4924</v>
+      </c>
+      <c r="D2">
         <v>4.4939999999999998</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>2.7549999999999999</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>72.441000000000003</v>
       </c>
-      <c r="G2">
+      <c r="I2">
+        <v>21.787500000000001</v>
+      </c>
+      <c r="J2">
         <v>4.1310000000000002</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>2.4620000000000002</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="J2">
+      <c r="M2">
         <v>61.149000000000001</v>
       </c>
-      <c r="K2">
+      <c r="N2">
+        <v>51.01</v>
+      </c>
+      <c r="O2">
         <v>4.093</v>
       </c>
-      <c r="L2">
+      <c r="P2">
         <v>7.9820000000000002</v>
       </c>
-      <c r="M2">
+      <c r="Q2">
         <v>1</v>
       </c>
-      <c r="N2">
+      <c r="R2">
         <v>53.804000000000002</v>
       </c>
-      <c r="O2">
+      <c r="S2">
+        <v>46.749000000000002</v>
+      </c>
+      <c r="T2">
         <v>4.1429999999999998</v>
       </c>
-      <c r="P2">
+      <c r="U2">
         <v>11.567</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:21">
       <c r="A3">
         <v>2</v>
       </c>
@@ -572,49 +612,61 @@
         <v>58.476999999999997</v>
       </c>
       <c r="C3">
+        <v>28.107399999999998</v>
+      </c>
+      <c r="D3">
         <v>4.2649999999999997</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>18.831</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>59.012</v>
       </c>
-      <c r="G3">
+      <c r="I3">
+        <v>27.627600000000001</v>
+      </c>
+      <c r="J3">
         <v>3.9169999999999998</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>20.463999999999999</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>2</v>
       </c>
-      <c r="J3">
+      <c r="M3">
         <v>58.750999999999998</v>
       </c>
-      <c r="K3">
+      <c r="N3">
+        <v>51.966099999999997</v>
+      </c>
+      <c r="O3">
         <v>5.7850000000000001</v>
       </c>
-      <c r="L3">
+      <c r="P3">
         <v>53.893000000000001</v>
       </c>
-      <c r="M3">
+      <c r="Q3">
         <v>2</v>
       </c>
-      <c r="N3">
+      <c r="R3">
         <v>62.180999999999997</v>
       </c>
-      <c r="O3">
+      <c r="S3">
+        <v>49.030299999999997</v>
+      </c>
+      <c r="T3">
         <v>6.7789999999999999</v>
       </c>
-      <c r="P3">
+      <c r="U3">
         <v>71.278000000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:21">
       <c r="A4">
         <v>3</v>
       </c>
@@ -622,49 +674,61 @@
         <v>51.363</v>
       </c>
       <c r="C4">
+        <v>26.7027</v>
+      </c>
+      <c r="D4">
         <v>4.6230000000000002</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>54.000999999999998</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>3</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>53.192999999999998</v>
       </c>
-      <c r="G4">
+      <c r="I4">
+        <v>30.9574</v>
+      </c>
+      <c r="J4">
         <v>4.4530000000000003</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>71.022999999999996</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>3</v>
       </c>
-      <c r="J4">
+      <c r="M4">
         <v>45.625999999999998</v>
       </c>
-      <c r="K4">
+      <c r="N4">
+        <v>42.461599999999997</v>
+      </c>
+      <c r="O4">
         <v>8.7309999999999999</v>
       </c>
-      <c r="L4">
+      <c r="P4">
         <v>139.54599999999999</v>
       </c>
-      <c r="M4">
+      <c r="Q4">
         <v>3</v>
       </c>
-      <c r="N4">
+      <c r="R4">
         <v>44.962000000000003</v>
       </c>
-      <c r="O4">
+      <c r="S4">
+        <v>37.927500000000002</v>
+      </c>
+      <c r="T4">
         <v>11.788</v>
       </c>
-      <c r="P4">
+      <c r="U4">
         <v>166.84899999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:21">
       <c r="A5">
         <v>4</v>
       </c>
@@ -672,49 +736,61 @@
         <v>37.817</v>
       </c>
       <c r="C5">
+        <v>24.6752</v>
+      </c>
+      <c r="D5">
         <v>4.66</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>89.787999999999997</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>4</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>37.973999999999997</v>
       </c>
-      <c r="G5">
+      <c r="I5">
+        <v>24.5717</v>
+      </c>
+      <c r="J5">
         <v>5.4260000000000002</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>130.48699999999999</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>4</v>
       </c>
-      <c r="J5">
+      <c r="M5">
         <v>34.963000000000001</v>
       </c>
-      <c r="K5">
+      <c r="N5">
+        <v>30.989599999999999</v>
+      </c>
+      <c r="O5">
         <v>14.022</v>
       </c>
-      <c r="L5">
+      <c r="P5">
         <v>249.51300000000001</v>
       </c>
-      <c r="M5">
+      <c r="Q5">
         <v>4</v>
       </c>
-      <c r="N5">
+      <c r="R5">
         <v>31.428000000000001</v>
       </c>
-      <c r="O5">
+      <c r="S5">
+        <v>25.770800000000001</v>
+      </c>
+      <c r="T5">
         <v>24.402000000000001</v>
       </c>
-      <c r="P5">
+      <c r="U5">
         <v>274.822</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:21">
       <c r="A6">
         <v>5</v>
       </c>
@@ -722,49 +798,61 @@
         <v>32.892000000000003</v>
       </c>
       <c r="C6">
+        <v>22.464099999999998</v>
+      </c>
+      <c r="D6">
         <v>4.6210000000000004</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>107.642</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>31.117000000000001</v>
       </c>
-      <c r="G6">
+      <c r="I6">
+        <v>19.4817</v>
+      </c>
+      <c r="J6">
         <v>4.375</v>
       </c>
-      <c r="H6">
+      <c r="K6">
         <v>165.10900000000001</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>5</v>
       </c>
-      <c r="J6">
+      <c r="M6">
         <v>25.471</v>
       </c>
-      <c r="K6">
+      <c r="N6">
+        <v>23.3659</v>
+      </c>
+      <c r="O6">
         <v>25.254999999999999</v>
       </c>
-      <c r="L6">
+      <c r="P6">
         <v>301.83</v>
       </c>
-      <c r="M6">
+      <c r="Q6">
         <v>5</v>
       </c>
-      <c r="N6">
+      <c r="R6">
         <v>24.251999999999999</v>
       </c>
-      <c r="O6">
+      <c r="S6">
+        <v>20.9222</v>
+      </c>
+      <c r="T6">
         <v>49.476999999999997</v>
       </c>
-      <c r="P6">
+      <c r="U6">
         <v>331.45</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:21">
       <c r="A7">
         <v>6</v>
       </c>
@@ -772,49 +860,61 @@
         <v>31.393000000000001</v>
       </c>
       <c r="C7">
+        <v>19.377199999999998</v>
+      </c>
+      <c r="D7">
         <v>3.8919999999999999</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>126.78</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>29.815000000000001</v>
       </c>
-      <c r="G7">
+      <c r="I7">
+        <v>18.174800000000001</v>
+      </c>
+      <c r="J7">
         <v>3.3650000000000002</v>
       </c>
-      <c r="H7">
+      <c r="K7">
         <v>194.93899999999999</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <v>6</v>
       </c>
-      <c r="J7">
+      <c r="M7">
         <v>25.145</v>
       </c>
-      <c r="K7">
+      <c r="N7">
+        <v>21.9086</v>
+      </c>
+      <c r="O7">
         <v>49.935000000000002</v>
       </c>
-      <c r="L7">
+      <c r="P7">
         <v>372.25799999999998</v>
       </c>
-      <c r="M7">
+      <c r="Q7">
         <v>6</v>
       </c>
-      <c r="N7">
+      <c r="R7">
         <v>25.558</v>
       </c>
-      <c r="O7">
+      <c r="S7">
+        <v>18.7776</v>
+      </c>
+      <c r="T7">
         <v>97.914000000000001</v>
       </c>
-      <c r="P7">
+      <c r="U7">
         <v>412.83600000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:21">
       <c r="A8">
         <v>7</v>
       </c>
@@ -822,49 +922,61 @@
         <v>24.811</v>
       </c>
       <c r="C8">
+        <v>19.183700000000002</v>
+      </c>
+      <c r="D8">
         <v>3.9039999999999999</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>112.949</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>7</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>22.172999999999998</v>
       </c>
-      <c r="G8">
+      <c r="I8">
+        <v>15.25</v>
+      </c>
+      <c r="J8">
         <v>4.6449999999999996</v>
       </c>
-      <c r="H8">
+      <c r="K8">
         <v>170.833</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <v>7</v>
       </c>
-      <c r="J8">
+      <c r="M8">
         <v>22.27</v>
       </c>
-      <c r="K8">
+      <c r="N8">
+        <v>20.2134</v>
+      </c>
+      <c r="O8">
         <v>78.087000000000003</v>
       </c>
-      <c r="L8">
+      <c r="P8">
         <v>353.31099999999998</v>
       </c>
-      <c r="M8">
+      <c r="Q8">
         <v>7</v>
       </c>
-      <c r="N8">
+      <c r="R8">
         <v>22.495000000000001</v>
       </c>
-      <c r="O8">
+      <c r="S8">
+        <v>17.064399999999999</v>
+      </c>
+      <c r="T8">
         <v>143.239</v>
       </c>
-      <c r="P8">
+      <c r="U8">
         <v>407.05700000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:21">
       <c r="A9">
         <v>8</v>
       </c>
@@ -872,49 +984,61 @@
         <v>29.884</v>
       </c>
       <c r="C9">
+        <v>16.1646</v>
+      </c>
+      <c r="D9">
         <v>4.3680000000000003</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>113.6</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>8</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>22.707999999999998</v>
       </c>
-      <c r="G9">
+      <c r="I9">
+        <v>14.5649</v>
+      </c>
+      <c r="J9">
         <v>4.29</v>
       </c>
-      <c r="H9">
+      <c r="K9">
         <v>167.48699999999999</v>
       </c>
-      <c r="I9">
+      <c r="L9">
         <v>8</v>
       </c>
-      <c r="J9">
+      <c r="M9">
         <v>20.27</v>
       </c>
-      <c r="K9">
+      <c r="N9">
+        <v>18.957799999999999</v>
+      </c>
+      <c r="O9">
         <v>101.77200000000001</v>
       </c>
-      <c r="L9">
+      <c r="P9">
         <v>319.88400000000001</v>
       </c>
-      <c r="M9">
+      <c r="Q9">
         <v>8</v>
       </c>
-      <c r="N9">
+      <c r="R9">
         <v>17.989999999999998</v>
       </c>
-      <c r="O9">
+      <c r="S9">
+        <v>16.921700000000001</v>
+      </c>
+      <c r="T9">
         <v>168.62700000000001</v>
       </c>
-      <c r="P9">
+      <c r="U9">
         <v>351.10399999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:21">
       <c r="A10">
         <v>9</v>
       </c>
@@ -922,49 +1046,61 @@
         <v>22.376000000000001</v>
       </c>
       <c r="C10">
+        <v>14.8301</v>
+      </c>
+      <c r="D10">
         <v>1.879</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>93.739000000000004</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>9</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>18.686</v>
       </c>
-      <c r="G10">
+      <c r="I10">
+        <v>10.4693</v>
+      </c>
+      <c r="J10">
         <v>1.986</v>
       </c>
-      <c r="H10">
+      <c r="K10">
         <v>145.923</v>
       </c>
-      <c r="I10">
+      <c r="L10">
         <v>10</v>
       </c>
-      <c r="J10">
+      <c r="M10">
         <v>21.413</v>
       </c>
-      <c r="K10">
+      <c r="N10">
+        <v>17.836500000000001</v>
+      </c>
+      <c r="O10">
         <v>161.46799999999999</v>
       </c>
-      <c r="L10">
+      <c r="P10">
         <v>256.334</v>
       </c>
-      <c r="M10">
+      <c r="Q10">
         <v>9</v>
       </c>
-      <c r="N10">
+      <c r="R10">
         <v>21.773</v>
       </c>
-      <c r="O10">
+      <c r="S10">
+        <v>12.850199999999999</v>
+      </c>
+      <c r="T10">
         <v>223.77099999999999</v>
       </c>
-      <c r="P10">
+      <c r="U10">
         <v>318.46899999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:21">
       <c r="A11">
         <v>10</v>
       </c>
@@ -972,49 +1108,61 @@
         <v>21.234999999999999</v>
       </c>
       <c r="C11">
+        <v>14.6777</v>
+      </c>
+      <c r="D11">
         <v>1.827</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>90.784000000000006</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>10</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>17.64</v>
       </c>
-      <c r="G11">
+      <c r="I11">
+        <v>9.7546999999999997</v>
+      </c>
+      <c r="J11">
         <v>1.788</v>
       </c>
-      <c r="H11">
+      <c r="K11">
         <v>138.541</v>
       </c>
-      <c r="I11">
+      <c r="L11">
         <v>11</v>
       </c>
-      <c r="J11">
+      <c r="M11">
         <v>20.695</v>
       </c>
-      <c r="K11">
+      <c r="N11">
+        <v>17.126000000000001</v>
+      </c>
+      <c r="O11">
         <v>179.732</v>
       </c>
-      <c r="L11">
+      <c r="P11">
         <v>219.09100000000001</v>
       </c>
-      <c r="M11">
+      <c r="Q11">
         <v>10</v>
       </c>
-      <c r="N11">
+      <c r="R11">
         <v>19.814</v>
       </c>
-      <c r="O11">
+      <c r="S11">
+        <v>14.3558</v>
+      </c>
+      <c r="T11">
         <v>244.172</v>
       </c>
-      <c r="P11">
+      <c r="U11">
         <v>265.36399999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:21">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1022,49 +1170,61 @@
         <v>19.861000000000001</v>
       </c>
       <c r="C12">
+        <v>12.7807</v>
+      </c>
+      <c r="D12">
         <v>1.7470000000000001</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>91.195999999999998</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>11</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>19.012</v>
       </c>
-      <c r="G12">
+      <c r="I12">
+        <v>14.2843</v>
+      </c>
+      <c r="J12">
         <v>1.885</v>
       </c>
-      <c r="H12">
+      <c r="K12">
         <v>141.60900000000001</v>
       </c>
-      <c r="I12">
+      <c r="L12">
         <v>12</v>
       </c>
-      <c r="J12">
+      <c r="M12">
         <v>23.896000000000001</v>
       </c>
-      <c r="K12">
+      <c r="N12">
+        <v>16.766300000000001</v>
+      </c>
+      <c r="O12">
         <v>228.066</v>
       </c>
-      <c r="L12">
+      <c r="P12">
         <v>226.53800000000001</v>
       </c>
-      <c r="M12">
+      <c r="Q12">
         <v>11</v>
       </c>
-      <c r="N12">
+      <c r="R12">
         <v>19.356000000000002</v>
       </c>
-      <c r="O12">
+      <c r="S12">
+        <v>15.419600000000001</v>
+      </c>
+      <c r="T12">
         <v>300.255</v>
       </c>
-      <c r="P12">
+      <c r="U12">
         <v>257.80399999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:21">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1072,49 +1232,61 @@
         <v>18.355</v>
       </c>
       <c r="C13">
+        <v>11.209899999999999</v>
+      </c>
+      <c r="D13">
         <v>1.7789999999999999</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>87.111999999999995</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>12</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>16.452999999999999</v>
       </c>
-      <c r="G13">
+      <c r="I13">
+        <v>8.5975900000000003</v>
+      </c>
+      <c r="J13">
         <v>2.21</v>
       </c>
-      <c r="H13">
+      <c r="K13">
         <v>120.575</v>
       </c>
-      <c r="I13">
+      <c r="L13">
         <v>14</v>
       </c>
-      <c r="J13">
+      <c r="M13">
         <v>19.291</v>
       </c>
-      <c r="K13">
+      <c r="N13">
+        <v>15.571099999999999</v>
+      </c>
+      <c r="O13">
         <v>209.292</v>
       </c>
-      <c r="L13">
+      <c r="P13">
         <v>137.697</v>
       </c>
-      <c r="M13">
+      <c r="Q13">
         <v>12</v>
       </c>
-      <c r="N13">
+      <c r="R13">
         <v>19.225999999999999</v>
       </c>
-      <c r="O13">
+      <c r="S13">
+        <v>14.919600000000001</v>
+      </c>
+      <c r="T13">
         <v>323.41899999999998</v>
       </c>
-      <c r="P13">
+      <c r="U13">
         <v>218.70099999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:21">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1122,49 +1294,61 @@
         <v>17.603999999999999</v>
       </c>
       <c r="C14">
+        <v>10.770799999999999</v>
+      </c>
+      <c r="D14">
         <v>2.157</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>90.206999999999994</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>13</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>16.452999999999999</v>
       </c>
-      <c r="G14">
+      <c r="I14">
+        <v>8.0835699999999999</v>
+      </c>
+      <c r="J14">
         <v>2.4390000000000001</v>
       </c>
-      <c r="H14">
+      <c r="K14">
         <v>117.286</v>
       </c>
-      <c r="I14">
+      <c r="L14">
         <v>15</v>
       </c>
-      <c r="J14">
+      <c r="M14">
         <v>18.472999999999999</v>
       </c>
-      <c r="K14">
+      <c r="N14">
+        <v>16.0351</v>
+      </c>
+      <c r="O14">
         <v>214.834</v>
       </c>
-      <c r="L14">
+      <c r="P14">
         <v>121.232</v>
       </c>
-      <c r="M14">
+      <c r="Q14">
         <v>13</v>
       </c>
-      <c r="N14">
+      <c r="R14">
         <v>18.539000000000001</v>
       </c>
-      <c r="O14">
+      <c r="S14">
+        <v>14.251300000000001</v>
+      </c>
+      <c r="T14">
         <v>341.55399999999997</v>
       </c>
-      <c r="P14">
+      <c r="U14">
         <v>186.172</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:21">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1172,49 +1356,61 @@
         <v>17.408999999999999</v>
       </c>
       <c r="C15">
+        <v>10.2004</v>
+      </c>
+      <c r="D15">
         <v>2.089</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>86.668000000000006</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>14</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <v>14.98</v>
       </c>
-      <c r="G15">
+      <c r="I15">
+        <v>7.3365600000000004</v>
+      </c>
+      <c r="J15">
         <v>1.736</v>
       </c>
-      <c r="H15">
+      <c r="K15">
         <v>104.974</v>
       </c>
-      <c r="I15">
+      <c r="L15">
         <v>16</v>
       </c>
-      <c r="J15">
+      <c r="M15">
         <v>17.853000000000002</v>
       </c>
-      <c r="K15">
+      <c r="N15">
+        <v>14.696400000000001</v>
+      </c>
+      <c r="O15">
         <v>217.06399999999999</v>
       </c>
-      <c r="L15">
+      <c r="P15">
         <v>103.111</v>
       </c>
-      <c r="M15">
+      <c r="Q15">
         <v>14</v>
       </c>
-      <c r="N15">
+      <c r="R15">
         <v>18.114000000000001</v>
       </c>
-      <c r="O15">
+      <c r="S15">
+        <v>14.8459</v>
+      </c>
+      <c r="T15">
         <v>380.27199999999999</v>
       </c>
-      <c r="P15">
+      <c r="U15">
         <v>147.624</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:21">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1222,49 +1418,61 @@
         <v>15.87</v>
       </c>
       <c r="C16">
+        <v>9.2065999999999999</v>
+      </c>
+      <c r="D16">
         <v>1.9730000000000001</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>83.751999999999995</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>15</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <v>14.914999999999999</v>
       </c>
-      <c r="G16">
+      <c r="I16">
+        <v>6.1617699999999997</v>
+      </c>
+      <c r="J16">
         <v>2.3420000000000001</v>
       </c>
-      <c r="H16">
+      <c r="K16">
         <v>103.33</v>
       </c>
-      <c r="I16">
+      <c r="L16">
         <v>17</v>
       </c>
-      <c r="J16">
+      <c r="M16">
         <v>17.690000000000001</v>
       </c>
-      <c r="K16">
+      <c r="N16">
+        <v>15.151199999999999</v>
+      </c>
+      <c r="O16">
         <v>214.32599999999999</v>
       </c>
-      <c r="L16">
+      <c r="P16">
         <v>83.819000000000003</v>
       </c>
-      <c r="M16">
+      <c r="Q16">
         <v>15</v>
       </c>
-      <c r="N16">
+      <c r="R16">
         <v>18.082000000000001</v>
       </c>
-      <c r="O16">
+      <c r="S16">
+        <v>15.0213</v>
+      </c>
+      <c r="T16">
         <v>389.30399999999997</v>
       </c>
-      <c r="P16">
+      <c r="U16">
         <v>118.959</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:21">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1272,49 +1480,61 @@
         <v>15.906000000000001</v>
       </c>
       <c r="C17">
+        <v>8.4455600000000004</v>
+      </c>
+      <c r="D17">
         <v>2.3519999999999999</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>91.195999999999998</v>
       </c>
-      <c r="E17">
+      <c r="G17">
         <v>16</v>
       </c>
-      <c r="F17">
+      <c r="H17">
         <v>14.167</v>
       </c>
-      <c r="G17">
+      <c r="I17">
+        <v>5.6401500000000002</v>
+      </c>
+      <c r="J17">
         <v>1.762</v>
       </c>
-      <c r="H17">
+      <c r="K17">
         <v>108.49</v>
       </c>
-      <c r="I17">
+      <c r="L17">
         <v>19</v>
       </c>
-      <c r="J17">
+      <c r="M17">
         <v>17.135000000000002</v>
       </c>
-      <c r="K17">
+      <c r="N17">
+        <v>14.2631</v>
+      </c>
+      <c r="O17">
         <v>220.12799999999999</v>
       </c>
-      <c r="L17">
+      <c r="P17">
         <v>55.185000000000002</v>
       </c>
-      <c r="M17">
+      <c r="Q17">
         <v>16</v>
       </c>
-      <c r="N17">
+      <c r="R17">
         <v>18.963999999999999</v>
       </c>
-      <c r="O17">
+      <c r="S17">
+        <v>15.141</v>
+      </c>
+      <c r="T17">
         <v>394.06200000000001</v>
       </c>
-      <c r="P17">
+      <c r="U17">
         <v>102.721</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:21">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1322,49 +1542,61 @@
         <v>14.954000000000001</v>
       </c>
       <c r="C18">
+        <v>7.1874099999999999</v>
+      </c>
+      <c r="D18">
         <v>1.6950000000000001</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>88.978999999999999</v>
       </c>
-      <c r="E18">
+      <c r="G18">
         <v>17</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <v>13.804</v>
       </c>
-      <c r="G18">
+      <c r="I18">
+        <v>4.9154999999999998</v>
+      </c>
+      <c r="J18">
         <v>1.879</v>
       </c>
-      <c r="H18">
+      <c r="K18">
         <v>108.203</v>
       </c>
-      <c r="I18">
+      <c r="L18">
         <v>20</v>
       </c>
-      <c r="J18">
+      <c r="M18">
         <v>18.963000000000001</v>
       </c>
-      <c r="K18">
+      <c r="N18">
+        <v>14.9282</v>
+      </c>
+      <c r="O18">
         <v>213.39599999999999</v>
       </c>
-      <c r="L18">
+      <c r="P18">
         <v>41.613</v>
       </c>
-      <c r="M18">
+      <c r="Q18">
         <v>17</v>
       </c>
-      <c r="N18">
+      <c r="R18">
         <v>18.146999999999998</v>
       </c>
-      <c r="O18">
+      <c r="S18">
+        <v>14.7614</v>
+      </c>
+      <c r="T18">
         <v>389.52300000000002</v>
       </c>
-      <c r="P18">
+      <c r="U18">
         <v>85.873999999999995</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:21">
       <c r="A19">
         <v>19</v>
       </c>
@@ -1372,49 +1604,61 @@
         <v>14.593</v>
       </c>
       <c r="C19">
+        <v>6.6186100000000003</v>
+      </c>
+      <c r="D19">
         <v>2.093</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>95.555999999999997</v>
       </c>
-      <c r="E19">
+      <c r="G19">
         <v>19</v>
       </c>
-      <c r="F19">
+      <c r="H19">
         <v>13.315</v>
       </c>
-      <c r="G19">
+      <c r="I19">
+        <v>4.1697600000000001</v>
+      </c>
+      <c r="J19">
         <v>1.74</v>
       </c>
-      <c r="H19">
+      <c r="K19">
         <v>112.099</v>
       </c>
-      <c r="I19">
+      <c r="L19">
         <v>21</v>
       </c>
-      <c r="J19">
+      <c r="M19">
         <v>18.356999999999999</v>
       </c>
-      <c r="K19">
+      <c r="N19">
+        <v>12.5626</v>
+      </c>
+      <c r="O19">
         <v>196.15700000000001</v>
       </c>
-      <c r="L19">
+      <c r="P19">
         <v>35.703000000000003</v>
       </c>
-      <c r="M19">
+      <c r="Q19">
         <v>19</v>
       </c>
-      <c r="N19">
+      <c r="R19">
         <v>18.18</v>
       </c>
-      <c r="O19">
+      <c r="S19">
+        <v>12.0756</v>
+      </c>
+      <c r="T19">
         <v>406.49099999999999</v>
       </c>
-      <c r="P19">
+      <c r="U19">
         <v>53.536999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:21">
       <c r="A20">
         <v>20</v>
       </c>
@@ -1422,49 +1666,61 @@
         <v>12.012</v>
       </c>
       <c r="C20">
+        <v>5.1565399999999997</v>
+      </c>
+      <c r="D20">
         <v>9.0869999999999997</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>78.564999999999998</v>
       </c>
-      <c r="E20">
+      <c r="G20">
         <v>20</v>
       </c>
-      <c r="F20">
+      <c r="H20">
         <v>12.763</v>
       </c>
-      <c r="G20">
+      <c r="I20">
+        <v>7.5465400000000002</v>
+      </c>
+      <c r="J20">
         <v>2.5139999999999998</v>
       </c>
-      <c r="H20">
+      <c r="K20">
         <v>110.54900000000001</v>
       </c>
-      <c r="I20">
+      <c r="L20">
         <v>22</v>
       </c>
-      <c r="J20">
+      <c r="M20">
         <v>18.356999999999999</v>
       </c>
-      <c r="K20">
+      <c r="N20">
+        <v>13.553800000000001</v>
+      </c>
+      <c r="O20">
         <v>197.38800000000001</v>
       </c>
-      <c r="L20">
+      <c r="P20">
         <v>30.4</v>
       </c>
-      <c r="M20">
+      <c r="Q20">
         <v>20</v>
       </c>
-      <c r="N20">
+      <c r="R20">
         <v>13.029</v>
       </c>
-      <c r="O20">
+      <c r="S20">
+        <v>11.2165</v>
+      </c>
+      <c r="T20">
         <v>244.00299999999999</v>
       </c>
-      <c r="P20">
+      <c r="U20">
         <v>24.853000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:21">
       <c r="A21">
         <v>21</v>
       </c>
@@ -1472,49 +1728,61 @@
         <v>13.803000000000001</v>
       </c>
       <c r="C21">
+        <v>4.2943199999999999</v>
+      </c>
+      <c r="D21">
         <v>3.0630000000000002</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>70</v>
       </c>
-      <c r="E21">
+      <c r="G21">
         <v>21</v>
       </c>
-      <c r="F21">
+      <c r="H21">
         <v>20.402000000000001</v>
       </c>
-      <c r="G21">
+      <c r="I21">
+        <v>9.4303100000000004</v>
+      </c>
+      <c r="J21">
         <v>1.5920000000000001</v>
       </c>
-      <c r="H21">
+      <c r="K21">
         <v>138.70400000000001</v>
       </c>
-      <c r="I21">
+      <c r="L21">
         <v>23</v>
       </c>
-      <c r="J21">
+      <c r="M21">
         <v>17.91</v>
       </c>
-      <c r="K21">
+      <c r="N21">
+        <v>14.0669</v>
+      </c>
+      <c r="O21">
         <v>192.83699999999999</v>
       </c>
-      <c r="L21">
+      <c r="P21">
         <v>25.306999999999999</v>
       </c>
-      <c r="M21">
+      <c r="Q21">
         <v>21</v>
       </c>
-      <c r="N21">
+      <c r="R21">
         <v>15.239000000000001</v>
       </c>
-      <c r="O21">
+      <c r="S21">
+        <v>5.4420099999999998</v>
+      </c>
+      <c r="T21">
         <v>2.3220000000000001</v>
       </c>
-      <c r="P21">
+      <c r="U21">
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:21">
       <c r="A22">
         <v>22</v>
       </c>
@@ -1522,49 +1790,61 @@
         <v>14.119</v>
       </c>
       <c r="C22">
+        <v>3.9249399999999999</v>
+      </c>
+      <c r="D22">
         <v>1.466</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>66.581999999999994</v>
       </c>
-      <c r="E22">
+      <c r="G22">
         <v>22</v>
       </c>
-      <c r="F22">
+      <c r="H22">
         <v>22.158000000000001</v>
       </c>
-      <c r="G22">
+      <c r="I22">
+        <v>15.3809</v>
+      </c>
+      <c r="J22">
         <v>3.5139999999999998</v>
       </c>
-      <c r="H22">
+      <c r="K22">
         <v>148.36799999999999</v>
       </c>
-      <c r="I22">
+      <c r="L22">
         <v>24</v>
       </c>
-      <c r="J22">
+      <c r="M22">
         <v>17.878</v>
       </c>
-      <c r="K22">
+      <c r="N22">
+        <v>14.036300000000001</v>
+      </c>
+      <c r="O22">
         <v>189.62299999999999</v>
       </c>
-      <c r="L22">
+      <c r="P22">
         <v>21.731000000000002</v>
       </c>
-      <c r="M22">
+      <c r="Q22">
         <v>22</v>
       </c>
-      <c r="N22">
+      <c r="R22">
         <v>15.91</v>
       </c>
-      <c r="O22">
+      <c r="S22">
+        <v>9.4722500000000007</v>
+      </c>
+      <c r="T22">
         <v>1.992</v>
       </c>
-      <c r="P22">
+      <c r="U22">
         <v>20.146000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:21">
       <c r="A23">
         <v>23</v>
       </c>
@@ -1572,49 +1852,61 @@
         <v>14.407</v>
       </c>
       <c r="C23">
+        <v>3.3269799999999998</v>
+      </c>
+      <c r="D23">
         <v>1.659</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>71.263000000000005</v>
       </c>
-      <c r="E23">
+      <c r="G23">
         <v>23</v>
       </c>
-      <c r="F23">
+      <c r="H23">
         <v>22.2</v>
       </c>
-      <c r="G23">
+      <c r="I23">
+        <v>15.37</v>
+      </c>
+      <c r="J23">
         <v>1.96</v>
       </c>
-      <c r="H23">
+      <c r="K23">
         <v>185.13900000000001</v>
       </c>
-      <c r="I23">
+      <c r="L23">
         <v>26</v>
       </c>
-      <c r="J23">
+      <c r="M23">
         <v>18.102</v>
       </c>
-      <c r="K23">
+      <c r="N23">
+        <v>14.757999999999999</v>
+      </c>
+      <c r="O23">
         <v>201.93799999999999</v>
       </c>
-      <c r="L23">
+      <c r="P23">
         <v>16.577000000000002</v>
       </c>
-      <c r="M23">
+      <c r="Q23">
         <v>23</v>
       </c>
-      <c r="N23">
+      <c r="R23">
         <v>15.656000000000001</v>
       </c>
-      <c r="O23">
+      <c r="S23">
+        <v>9.2992100000000004</v>
+      </c>
+      <c r="T23">
         <v>1.9470000000000001</v>
       </c>
-      <c r="P23">
+      <c r="U23">
         <v>12.885</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:21">
       <c r="A24">
         <v>24</v>
       </c>
@@ -1622,49 +1914,61 @@
         <v>14.244</v>
       </c>
       <c r="C24">
+        <v>3.1090200000000001</v>
+      </c>
+      <c r="D24">
         <v>1.571</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>70.238</v>
       </c>
-      <c r="E24">
+      <c r="G24">
         <v>24</v>
       </c>
-      <c r="F24">
+      <c r="H24">
         <v>20.602</v>
       </c>
-      <c r="G24">
+      <c r="I24">
+        <v>13.7241</v>
+      </c>
+      <c r="J24">
         <v>3.6349999999999998</v>
       </c>
-      <c r="H24">
+      <c r="K24">
         <v>212.37799999999999</v>
       </c>
-      <c r="I24">
+      <c r="L24">
         <v>27</v>
       </c>
-      <c r="J24">
+      <c r="M24">
         <v>17.686</v>
       </c>
-      <c r="K24">
+      <c r="N24">
+        <v>13.972799999999999</v>
+      </c>
+      <c r="O24">
         <v>203.81700000000001</v>
       </c>
-      <c r="L24">
+      <c r="P24">
         <v>14.021000000000001</v>
       </c>
-      <c r="M24">
+      <c r="Q24">
         <v>24</v>
       </c>
-      <c r="N24">
+      <c r="R24">
         <v>16.196999999999999</v>
       </c>
-      <c r="O24">
+      <c r="S24">
+        <v>10.2791</v>
+      </c>
+      <c r="T24">
         <v>2.02</v>
       </c>
-      <c r="P24">
+      <c r="U24">
         <v>11.441000000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:21">
       <c r="A25">
         <v>26</v>
       </c>
@@ -1672,49 +1976,61 @@
         <v>14.055</v>
       </c>
       <c r="C25">
+        <v>2.97871</v>
+      </c>
+      <c r="D25">
         <v>2.0110000000000001</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>63.847999999999999</v>
       </c>
-      <c r="E25">
+      <c r="G25">
         <v>26</v>
       </c>
-      <c r="F25">
+      <c r="H25">
         <v>17.856999999999999</v>
       </c>
-      <c r="G25">
+      <c r="I25">
+        <v>11.4536</v>
+      </c>
+      <c r="J25">
         <v>53.88</v>
       </c>
-      <c r="H25">
+      <c r="K25">
         <v>198.68299999999999</v>
       </c>
-      <c r="I25">
+      <c r="L25">
         <v>28</v>
       </c>
-      <c r="J25">
+      <c r="M25">
         <v>18.420000000000002</v>
       </c>
-      <c r="K25">
+      <c r="N25">
+        <v>14.402900000000001</v>
+      </c>
+      <c r="O25">
         <v>222.35900000000001</v>
       </c>
-      <c r="L25">
+      <c r="P25">
         <v>12.502000000000001</v>
       </c>
-      <c r="M25">
+      <c r="Q25">
         <v>26</v>
       </c>
-      <c r="N25">
+      <c r="R25">
         <v>16.071000000000002</v>
       </c>
-      <c r="O25">
+      <c r="S25">
+        <v>9.7726199999999999</v>
+      </c>
+      <c r="T25">
         <v>2.024</v>
       </c>
-      <c r="P25">
+      <c r="U25">
         <v>8.968</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:21">
       <c r="A26">
         <v>27</v>
       </c>
@@ -1722,49 +2038,61 @@
         <v>13.000999999999999</v>
       </c>
       <c r="C26">
+        <v>2.4324400000000002</v>
+      </c>
+      <c r="D26">
         <v>1.663</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>51.314999999999998</v>
       </c>
-      <c r="E26">
+      <c r="G26">
         <v>27</v>
       </c>
-      <c r="F26">
+      <c r="H26">
         <v>18.484999999999999</v>
       </c>
-      <c r="G26">
+      <c r="I26">
+        <v>11.1153</v>
+      </c>
+      <c r="J26">
         <v>70.076999999999998</v>
       </c>
-      <c r="H26">
+      <c r="K26">
         <v>188.16300000000001</v>
       </c>
-      <c r="I26">
+      <c r="L26">
         <v>29</v>
       </c>
-      <c r="J26">
+      <c r="M26">
         <v>18.484000000000002</v>
       </c>
-      <c r="K26">
+      <c r="N26">
+        <v>14.692</v>
+      </c>
+      <c r="O26">
         <v>242.82</v>
       </c>
-      <c r="L26">
+      <c r="P26">
         <v>10.214</v>
       </c>
-      <c r="M26">
+      <c r="Q26">
         <v>27</v>
       </c>
-      <c r="N26">
+      <c r="R26">
         <v>14.792</v>
       </c>
-      <c r="O26">
+      <c r="S26">
+        <v>8.4503799999999991</v>
+      </c>
+      <c r="T26">
         <v>4.2069999999999999</v>
       </c>
-      <c r="P26">
+      <c r="U26">
         <v>7.2489999999999997</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:21">
       <c r="A27">
         <v>28</v>
       </c>
@@ -1772,49 +2100,61 @@
         <v>13.417</v>
       </c>
       <c r="C27">
+        <v>2.38924</v>
+      </c>
+      <c r="D27">
         <v>2.629</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>52.49</v>
       </c>
-      <c r="E27">
+      <c r="G27">
         <v>28</v>
       </c>
-      <c r="F27">
+      <c r="H27">
         <v>17.815000000000001</v>
       </c>
-      <c r="G27">
+      <c r="I27">
+        <v>10.5266</v>
+      </c>
+      <c r="J27">
         <v>115.024</v>
       </c>
-      <c r="H27">
+      <c r="K27">
         <v>158.51400000000001</v>
       </c>
-      <c r="I27">
+      <c r="L27">
         <v>31</v>
       </c>
-      <c r="J27">
+      <c r="M27">
         <v>18.486000000000001</v>
       </c>
-      <c r="K27">
+      <c r="N27">
+        <v>14.0726</v>
+      </c>
+      <c r="O27">
         <v>238.548</v>
       </c>
-      <c r="L27">
+      <c r="P27">
         <v>7.5540000000000003</v>
       </c>
-      <c r="M27">
+      <c r="Q27">
         <v>28</v>
       </c>
-      <c r="N27">
+      <c r="R27">
         <v>16.934000000000001</v>
       </c>
-      <c r="O27">
+      <c r="S27">
+        <v>10.3675</v>
+      </c>
+      <c r="T27">
         <v>1.869</v>
       </c>
-      <c r="P27">
+      <c r="U27">
         <v>8.0039999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:21">
       <c r="A28">
         <v>29</v>
       </c>
@@ -1822,49 +2162,61 @@
         <v>13.068</v>
       </c>
       <c r="C28">
+        <v>3.4887999999999999</v>
+      </c>
+      <c r="D28">
         <v>1.7649999999999999</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>52.430999999999997</v>
       </c>
-      <c r="E28">
+      <c r="G28">
         <v>29</v>
       </c>
-      <c r="F28">
+      <c r="H28">
         <v>17.655000000000001</v>
       </c>
-      <c r="G28">
+      <c r="I28">
+        <v>11.089600000000001</v>
+      </c>
+      <c r="J28">
         <v>165.34100000000001</v>
       </c>
-      <c r="H28">
+      <c r="K28">
         <v>132.74</v>
       </c>
-      <c r="I28">
+      <c r="L28">
         <v>33</v>
       </c>
-      <c r="J28">
+      <c r="M28">
         <v>18.835999999999999</v>
       </c>
-      <c r="K28">
+      <c r="N28">
+        <v>14.809200000000001</v>
+      </c>
+      <c r="O28">
         <v>243.453</v>
       </c>
-      <c r="L28">
+      <c r="P28">
         <v>6.0720000000000001</v>
       </c>
-      <c r="M28">
+      <c r="Q28">
         <v>29</v>
       </c>
-      <c r="N28">
+      <c r="R28">
         <v>15.178000000000001</v>
       </c>
-      <c r="O28">
+      <c r="S28">
+        <v>7.8329899999999997</v>
+      </c>
+      <c r="T28">
         <v>1.8839999999999999</v>
       </c>
-      <c r="P28">
+      <c r="U28">
         <v>6.5270000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:21">
       <c r="A29">
         <v>31</v>
       </c>
@@ -1872,49 +2224,61 @@
         <v>13.101000000000001</v>
       </c>
       <c r="C29">
+        <v>2.7979599999999998</v>
+      </c>
+      <c r="D29">
         <v>1.5289999999999999</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>48.037999999999997</v>
       </c>
-      <c r="E29">
+      <c r="G29">
         <v>31</v>
       </c>
-      <c r="F29">
+      <c r="H29">
         <v>16.666</v>
       </c>
-      <c r="G29">
+      <c r="I29">
+        <v>9.7034400000000005</v>
+      </c>
+      <c r="J29">
         <v>201.376</v>
       </c>
-      <c r="H29">
+      <c r="K29">
         <v>92.843999999999994</v>
       </c>
-      <c r="I29">
+      <c r="L29">
         <v>34</v>
       </c>
-      <c r="J29">
+      <c r="M29">
         <v>19.087</v>
       </c>
-      <c r="K29">
+      <c r="N29">
+        <v>14.718299999999999</v>
+      </c>
+      <c r="O29">
         <v>228.40199999999999</v>
       </c>
-      <c r="L29">
+      <c r="P29">
         <v>5.5549999999999997</v>
       </c>
-      <c r="M29">
+      <c r="Q29">
         <v>31</v>
       </c>
-      <c r="N29">
+      <c r="R29">
         <v>13.451000000000001</v>
       </c>
-      <c r="O29">
+      <c r="S29">
+        <v>5.2778400000000003</v>
+      </c>
+      <c r="T29">
         <v>2.4990000000000001</v>
       </c>
-      <c r="P29">
+      <c r="U29">
         <v>5.4560000000000004</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:21">
       <c r="A30">
         <v>33</v>
       </c>
@@ -1922,49 +2286,61 @@
         <v>12.621</v>
       </c>
       <c r="C30">
+        <v>2.06236</v>
+      </c>
+      <c r="D30">
         <v>2.9660000000000002</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>43.851999999999997</v>
       </c>
-      <c r="E30">
+      <c r="G30">
         <v>33</v>
       </c>
-      <c r="F30">
+      <c r="H30">
         <v>15.805</v>
       </c>
-      <c r="G30">
+      <c r="I30">
+        <v>8.7263500000000001</v>
+      </c>
+      <c r="J30">
         <v>222.34899999999999</v>
       </c>
-      <c r="H30">
+      <c r="K30">
         <v>64.153999999999996</v>
       </c>
-      <c r="I30">
+      <c r="L30">
         <v>35</v>
       </c>
-      <c r="J30">
+      <c r="M30">
         <v>19.606999999999999</v>
       </c>
-      <c r="K30">
+      <c r="N30">
+        <v>13.206200000000001</v>
+      </c>
+      <c r="O30">
         <v>222.452</v>
       </c>
-      <c r="L30">
+      <c r="P30">
         <v>5.2770000000000001</v>
       </c>
-      <c r="M30">
+      <c r="Q30">
         <v>33</v>
       </c>
-      <c r="N30">
+      <c r="R30">
         <v>13.772</v>
       </c>
-      <c r="O30">
+      <c r="S30">
+        <v>6.9188299999999998</v>
+      </c>
+      <c r="T30">
         <v>1.6619999999999999</v>
       </c>
-      <c r="P30">
+      <c r="U30">
         <v>5.2859999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:21">
       <c r="A31">
         <v>34</v>
       </c>
@@ -1972,37 +2348,46 @@
         <v>12.397</v>
       </c>
       <c r="C31">
+        <v>2.1406000000000001</v>
+      </c>
+      <c r="D31">
         <v>2.004</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>42.256</v>
       </c>
-      <c r="E31">
+      <c r="G31">
         <v>34</v>
       </c>
-      <c r="F31">
+      <c r="H31">
         <v>14.66</v>
       </c>
-      <c r="G31">
+      <c r="I31">
+        <v>8.32301</v>
+      </c>
+      <c r="J31">
         <v>216.41399999999999</v>
       </c>
-      <c r="H31">
+      <c r="K31">
         <v>48.475999999999999</v>
       </c>
-      <c r="M31">
+      <c r="Q31">
         <v>34</v>
       </c>
-      <c r="N31">
+      <c r="R31">
         <v>13.771000000000001</v>
       </c>
-      <c r="O31">
+      <c r="S31">
+        <v>6.3546500000000004</v>
+      </c>
+      <c r="T31">
         <v>1.7569999999999999</v>
       </c>
-      <c r="P31">
+      <c r="U31">
         <v>5.2</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:21">
       <c r="A32">
         <v>35</v>
       </c>
@@ -2010,33 +2395,42 @@
         <v>12.619</v>
       </c>
       <c r="C32">
+        <v>2.1567599999999998</v>
+      </c>
+      <c r="D32">
         <v>4.601</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>39.384</v>
       </c>
-      <c r="E32">
+      <c r="G32">
         <v>35</v>
       </c>
-      <c r="F32">
+      <c r="H32">
         <v>14.369</v>
       </c>
-      <c r="G32">
+      <c r="I32">
+        <v>7.5165600000000001</v>
+      </c>
+      <c r="J32">
         <v>225.071</v>
       </c>
-      <c r="H32">
+      <c r="K32">
         <v>38.951999999999998</v>
       </c>
-      <c r="M32">
+      <c r="Q32">
         <v>35</v>
       </c>
-      <c r="N32">
+      <c r="R32">
         <v>13.516</v>
       </c>
-      <c r="O32">
+      <c r="S32">
+        <v>7.3726500000000001</v>
+      </c>
+      <c r="T32">
         <v>1.8029999999999999</v>
       </c>
-      <c r="P32">
+      <c r="U32">
         <v>4.9480000000000004</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Electron balance and siderite SI calculations
One large worksheet showing values for siderite saturation and electron
balance with acetate/bicarbonate data for each aggregate reactor
</commit_message>
<xml_diff>
--- a/Aggregate_AqMnAsFe.xlsx
+++ b/Aggregate_AqMnAsFe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2920" yWindow="580" windowWidth="27140" windowHeight="17100" tabRatio="500"/>
+    <workbookView xWindow="1060" yWindow="2240" windowWidth="29440" windowHeight="16820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Tot1.25-bicarb1</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -94,6 +94,14 @@
   </si>
   <si>
     <t>siderite_SI_3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jensen et al.,2002. The solubility of rhodochrosite (MnCO3) and siderite (FeCO3) in anaerobic aquatic environments. Applied Geochemistry.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ksp value for siderite taken from:</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -631,8 +639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AZ74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AY51" sqref="AY51"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
@@ -651,37 +659,37 @@
   <sheetData>
     <row r="1" spans="1:52">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>5</v>
@@ -690,31 +698,31 @@
         <v>6</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>8</v>
@@ -726,34 +734,34 @@
         <v>10</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="AH1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="AJ1" s="1" t="s">
         <v>12</v>
@@ -768,31 +776,31 @@
         <v>0</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="AR1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="AU1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="AV1" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="AW1" s="1" t="s">
         <v>16</v>
@@ -804,7 +812,7 @@
         <v>18</v>
       </c>
       <c r="AZ1" s="1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:52">
@@ -6483,25 +6491,31 @@
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="38" spans="1:18">
+      <c r="A38" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
     </row>
     <row r="39" spans="1:18">
+      <c r="A39" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="Q39" s="2"/>
@@ -6720,6 +6734,7 @@
       <c r="P74" s="2"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>